<commit_message>
fix: Correct Excel products and inventory
</commit_message>
<xml_diff>
--- a/src/assets/modelo_crear_inventario.xlsx
+++ b/src/assets/modelo_crear_inventario.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27406"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="7" documentId="11_9248B46DC1CBB2E3ED7FF6F9903E8C1851038383" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{892AAF15-F498-477A-B712-13D2089035D2}"/>
+  <xr:revisionPtr revIDLastSave="94" documentId="11_9248B46DC1CBB2E3ED7FF6F9903E8C1851038383" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4FFCCFCB-EC66-4575-8877-7A64C66FE7E4}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,28 +33,34 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
-    <t>article</t>
+    <t>Código del producto</t>
   </si>
   <si>
-    <t>realStock</t>
+    <t>Stock real</t>
   </si>
   <si>
-    <t>minStock</t>
+    <t>Stock mínimo</t>
   </si>
   <si>
-    <t>maxStock</t>
+    <t>Stock máximo</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF212529"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -78,8 +84,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -394,16 +402,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="22" style="2" customWidth="1"/>
+    <col min="2" max="2" width="10" customWidth="1"/>
+    <col min="3" max="4" width="14" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
@@ -417,11 +430,18 @@
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2">
-        <v>898</v>
-      </c>
+      <c r="A2" s="1"/>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="1"/>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="1"/>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2" xr:uid="{6A306CFF-CD1C-4E27-BD16-2F44D4279F43}"/>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>